<commit_message>
table, create client, create venue, id for client
</commit_message>
<xml_diff>
--- a/src/res/sheets/The_Wedding_Planner.xlsx
+++ b/src/res/sheets/The_Wedding_Planner.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="749" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="35">
   <si>
     <t>ID</t>
   </si>
@@ -28,12 +28,12 @@
     <t>AccessLevel</t>
   </si>
   <si>
+    <t>VID</t>
+  </si>
+  <si>
     <t>Venue Name</t>
   </si>
   <si>
-    <t xml:space="preserve">VenueID </t>
-  </si>
-  <si>
     <t>Date</t>
   </si>
   <si>
@@ -46,7 +46,7 @@
     <t>Estimated Items Needed</t>
   </si>
   <si>
-    <t>ReservationID</t>
+    <t>RID</t>
   </si>
   <si>
     <t>Wedding Date</t>
@@ -58,15 +58,15 @@
     <t>Approximate Price</t>
   </si>
   <si>
+    <t>CID</t>
+  </si>
+  <si>
     <t>Name</t>
   </si>
   <si>
     <t>Date of Birth</t>
   </si>
   <si>
-    <t>Age</t>
-  </si>
-  <si>
     <t>Email</t>
   </si>
   <si>
@@ -79,43 +79,49 @@
     <t>Quantity</t>
   </si>
   <si>
-    <t>12</t>
-  </si>
-  <si>
-    <t>Richard</t>
-  </si>
-  <si>
-    <t>medium</t>
-  </si>
-  <si>
-    <t>13</t>
-  </si>
-  <si>
-    <t>Simon</t>
-  </si>
-  <si>
-    <t>low</t>
-  </si>
-  <si>
-    <t>Long Mountain</t>
-  </si>
-  <si>
-    <t>25</t>
-  </si>
-  <si>
-    <t>2021-02-27</t>
-  </si>
-  <si>
-    <t>Kingston</t>
-  </si>
-  <si>
-    <t>Roger</t>
-  </si>
-  <si>
-    <t>roger@gmail.com</t>
-  </si>
-  <si>
-    <t>1235555555</t>
+    <t>yo cok</t>
+  </si>
+  <si>
+    <t>2020-11-03</t>
+  </si>
+  <si>
+    <t>yocok@gmail.com</t>
+  </si>
+  <si>
+    <t>8764185312</t>
+  </si>
+  <si>
+    <t>cwilkins</t>
+  </si>
+  <si>
+    <t>2021-10-11</t>
+  </si>
+  <si>
+    <t>ckw@gmail.com</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>long cocky bro</t>
+  </si>
+  <si>
+    <t>2021-10-23</t>
+  </si>
+  <si>
+    <t>lcb@gmail.com</t>
+  </si>
+  <si>
+    <t>8769921134</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>2021-10-30</t>
   </si>
 </sst>
 </file>
@@ -160,14 +166,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="3.26953125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="7.80078125" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="2.9453125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="6.6875" collapsed="true"/>
     <col min="3" max="3" bestFit="true" customWidth="true" width="11.59765625" collapsed="true"/>
   </cols>
   <sheetData>
@@ -182,28 +188,6 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C3" t="s">
-        <v>25</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
@@ -211,17 +195,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="14.6171875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="9.19140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="11.3046875" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="4.1953125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="12.609375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="5.27734375" collapsed="true"/>
     <col min="4" max="4" bestFit="true" customWidth="true" width="11.6015625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="8.7890625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="8.6640625" collapsed="true"/>
     <col min="6" max="6" bestFit="true" customWidth="true" width="23.02734375" collapsed="true"/>
   </cols>
   <sheetData>
@@ -245,20 +229,6 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E2" t="s">
-        <v>29</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
@@ -272,7 +242,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="13.5625" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="4.140625" collapsed="true"/>
     <col min="2" max="2" bestFit="true" customWidth="true" width="13.83203125" collapsed="true"/>
     <col min="3" max="3" bestFit="true" customWidth="true" width="17.25" collapsed="true"/>
     <col min="4" max="4" bestFit="true" customWidth="true" width="17.58203125" collapsed="true"/>
@@ -299,16 +269,16 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="6.36328125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="12.46484375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="4.44140625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="17.08984375" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="4.1171875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="13.98828125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="12.46484375" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="17.51171875" collapsed="true"/>
     <col min="5" max="5" bestFit="true" customWidth="true" width="15.44921875" collapsed="true"/>
   </cols>
   <sheetData>
@@ -330,20 +300,71 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="s">
+      <c r="A2" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" t="s">
         <v>30</v>
       </c>
-      <c r="B2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C2" t="n">
-        <v>19.0</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="E4" t="s">
         <v>31</v>
       </c>
-      <c r="E2" t="s">
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
         <v>32</v>
+      </c>
+      <c r="B5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E5" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -386,7 +407,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B1" t="s">
         <v>19</v>

</xml_diff>

<commit_message>
After Presentation (Refer to previous comit)
</commit_message>
<xml_diff>
--- a/src/res/sheets/The_Wedding_Planner.xlsx
+++ b/src/res/sheets/The_Wedding_Planner.xlsx
@@ -1,29 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="9302"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24527"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent>
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chava\Desktop\School\Software Engineering\Project\TheWeddingPlanner\src\res\sheets\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{972A5544-3537-41E4-8B76-0ECDCF228DB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="120" windowWidth="14940" windowHeight="9225" firstSheet="4" activeTab="9"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11505" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="User" sheetId="1" r:id="rId3"/>
-    <sheet name="Venue" sheetId="2" r:id="rId4"/>
-    <sheet name="Inventory" sheetId="3" r:id="rId5"/>
-    <sheet name="Client" sheetId="4" r:id="rId6"/>
-    <sheet name="Reservation" sheetId="5" r:id="rId7"/>
-    <sheet name="Items" sheetId="6" r:id="rId8"/>
-    <sheet name="Evaluation Warning" sheetId="7" r:id="rId9"/>
-    <sheet name="Evaluation Warning (1)" sheetId="8" r:id="rId10"/>
-    <sheet name="Evaluation Warning (2)" sheetId="9" r:id="rId11"/>
-    <sheet name="Evaluation Warning (3)" sheetId="10" r:id="rId12"/>
+    <sheet name="User" sheetId="1" r:id="rId1"/>
+    <sheet name="Venue" sheetId="2" r:id="rId2"/>
+    <sheet name="Inventory" sheetId="3" r:id="rId3"/>
+    <sheet name="Client" sheetId="4" r:id="rId4"/>
+    <sheet name="Reservation" sheetId="5" r:id="rId5"/>
+    <sheet name="Items" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="690" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="837" uniqueCount="51">
   <si>
     <t>ID</t>
   </si>
@@ -76,74 +78,117 @@
     <t>Phone Numbers</t>
   </si>
   <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>Long Mountain</t>
+  </si>
+  <si>
+    <t>2021-02-27</t>
+  </si>
+  <si>
+    <t>Hotel</t>
+  </si>
+  <si>
+    <t>Kingston</t>
+  </si>
+  <si>
+    <t>Roger</t>
+  </si>
+  <si>
+    <t>roger@gmail.com</t>
+  </si>
+  <si>
+    <t>1235555555</t>
+  </si>
+  <si>
+    <t>Estimated Items Needed</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>Aloe Vera</t>
+  </si>
+  <si>
+    <t>2000-11-13</t>
+  </si>
+  <si>
+    <t>aloevera@hotmail.com</t>
+  </si>
+  <si>
+    <t>8764185312</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>2021-11-15</t>
+  </si>
+  <si>
+    <t>2021-11-29</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Luis Mitton Chair</t>
+  </si>
+  <si>
+    <t>250</t>
+  </si>
+  <si>
     <t>Chairs</t>
   </si>
   <si>
-    <t>Quantity</t>
-  </si>
-  <si>
-    <t>Evaluation Only. Created with Aspose.Cells for Java.Copyright 2003 - 2021 Aspose Pty Ltd.</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>Long Mountain</t>
-  </si>
-  <si>
-    <t>2021-02-27</t>
-  </si>
-  <si>
-    <t>Hotel</t>
-  </si>
-  <si>
-    <t>Kingston</t>
-  </si>
-  <si>
-    <t>Roger</t>
-  </si>
-  <si>
-    <t>roger@gmail.com</t>
-  </si>
-  <si>
-    <t>1235555555</t>
-  </si>
-  <si>
-    <t>Estimated Items Needed</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>Aloe Vera</t>
-  </si>
-  <si>
-    <t>2000-11-13</t>
-  </si>
-  <si>
-    <t>aloevera@hotmail.com</t>
-  </si>
-  <si>
-    <t>8764185312</t>
+    <t>2021-11-13</t>
+  </si>
+  <si>
+    <t>2021-11-24</t>
+  </si>
+  <si>
+    <t>Luis Chairs</t>
+  </si>
+  <si>
+    <t>26</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>International Water</t>
+  </si>
+  <si>
+    <t>2021-11-20</t>
+  </si>
+  <si>
+    <t>Waterfall</t>
+  </si>
+  <si>
+    <t>Saint Catherine</t>
+  </si>
+  <si>
+    <t>Sir John the third</t>
+  </si>
+  <si>
+    <t>2006-11-07</t>
+  </si>
+  <si>
+    <t>john@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <i/>
-      <sz val="18"/>
-      <color rgb="FF0000FF"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -165,117 +210,23 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
-      <alignment/>
-      <protection/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment/>
-      <protection/>
-    </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Percent" xfId="15" builtinId="5"/>
-    <cellStyle name="Currency" xfId="16" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="17" builtinId="7"/>
-    <cellStyle name="Comma" xfId="18" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="19" builtinId="6"/>
   </cellStyles>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -577,12 +528,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45b4c9bf-181f-4fd6-9d19-84298be9a80d}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45B4C9BF-181F-4FD6-9D19-84298BE9A80D}">
   <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView workbookViewId="0" topLeftCell="A1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" bestFit="true" customWidth="true" width="3.015625" collapsed="true"/>
     <col min="2" max="2" bestFit="true" customWidth="true" width="6.79296875" collapsed="true"/>
@@ -606,41 +557,19 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90ba0c6d-1baa-4ffe-af11-b1593476b4ac}">
-  <dimension ref="A5"/>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B81FECDD-389F-423C-8016-FFAE913CC65B}">
+  <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" topLeftCell="A1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
-  <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="157.703125" collapsed="true"/>
-  </cols>
-  <sheetData>
-    <row r="5" spans="1:1" ht="23.25" customHeight="1">
-      <c r="A5" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{b81fecdd-389f-423c-8016-ffae913cc65b}">
-  <dimension ref="A1:F2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0" topLeftCell="A1"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" bestFit="true" customWidth="true" width="4.3515625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="14.25" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="17.9140625" collapsed="true"/>
     <col min="3" max="3" bestFit="true" customWidth="true" width="11.24609375" collapsed="true"/>
     <col min="4" max="4" bestFit="true" customWidth="true" width="11.80078125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="8.80078125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="14.80078125" collapsed="true"/>
     <col min="6" max="6" bestFit="true" customWidth="true" width="22.9140625" collapsed="true"/>
   </cols>
   <sheetData>
@@ -661,24 +590,41 @@
         <v>7</v>
       </c>
       <c r="F1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="12.75">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" t="s">
         <v>20</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D2" t="s">
         <v>21</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
         <v>22</v>
       </c>
-      <c r="D2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E2" t="s">
-        <v>24</v>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E3" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -688,14 +634,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{b68495ad-f97a-4fc6-ac81-ca19a4e84e66}">
-  <dimension ref="A1:D1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B68495AD-F97A-4FC6-AC81-CA19A4E84E66}">
+  <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0" topLeftCell="A1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="4.4609375" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="16.0234375" collapsed="true"/>
     <col min="2" max="2" bestFit="true" customWidth="true" width="13.69140625" collapsed="true"/>
     <col min="3" max="3" bestFit="true" customWidth="true" width="17.46875" collapsed="true"/>
     <col min="4" max="4" bestFit="true" customWidth="true" width="17.35546875" collapsed="true"/>
@@ -715,6 +661,28 @@
         <v>11</v>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C3" t="s">
+        <v>38</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait"/>
@@ -722,15 +690,15 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97291122-8e8f-4d31-a955-92be2b1eb64a}">
-  <dimension ref="A1:E3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97291122-8E8F-4D31-A955-92BE2B1EB64A}">
+  <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView workbookViewId="0" topLeftCell="A1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" bestFit="true" customWidth="true" width="4.4609375" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="9.80078125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="16.13671875" collapsed="true"/>
     <col min="3" max="3" bestFit="true" customWidth="true" width="12.1328125" collapsed="true"/>
     <col min="4" max="4" bestFit="true" customWidth="true" width="21.5" collapsed="true"/>
     <col min="5" max="5" bestFit="true" customWidth="true" width="15.46875" collapsed="true"/>
@@ -753,38 +721,55 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="12.75">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" t="s">
         <v>20</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2" t="s">
         <v>25</v>
       </c>
-      <c r="C2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E2" t="s">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="s">
+      <c r="B3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" t="s">
         <v>29</v>
       </c>
-      <c r="B3" t="s">
+      <c r="D3" t="s">
         <v>30</v>
       </c>
-      <c r="C3" t="s">
+      <c r="E3" t="s">
         <v>31</v>
       </c>
-      <c r="D3" t="s">
-        <v>32</v>
-      </c>
-      <c r="E3" t="s">
-        <v>33</v>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E4" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -794,19 +779,56 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{c7b56dd0-638f-4c6e-9bdc-063d2af51841}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7B56DD0-638F-4C6E-9BDC-063D2AF51841}">
+  <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0" topLeftCell="A1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="6.796875" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="6.3515625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="11.24609375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="11.24609375" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="7.69140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" t="s">
         <v>17</v>
+      </c>
+      <c r="C1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2">
+        <v>555021</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D3" t="n">
+        <v>25000.0</v>
       </c>
     </row>
   </sheetData>
@@ -816,89 +838,23 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{685976c5-99ae-42aa-9eee-74533a8759b3}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{685976C5-99AE-42AA-9EEE-74533A8759B3}">
   <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView workbookViewId="0" topLeftCell="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" bestFit="true" customWidth="true" width="6.3515625" collapsed="true"/>
     <col min="2" max="2" bestFit="true" customWidth="true" width="8.46484375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>13</v>
       </c>
       <c r="B1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91c33aa4-9a2c-4b17-a1ef-e2babff9b9d0}">
-  <dimension ref="A5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0" topLeftCell="A1"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
-  <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="157.703125" collapsed="true"/>
-  </cols>
-  <sheetData>
-    <row r="5" spans="1:1" ht="23.25" customHeight="1">
-      <c r="A5" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ada90431-2c97-4156-a7cb-1ef594664a05}">
-  <dimension ref="A5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0" topLeftCell="A1"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
-  <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="157.703125" collapsed="true"/>
-  </cols>
-  <sheetData>
-    <row r="5" spans="1:1" ht="23.25" customHeight="1">
-      <c r="A5" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1a66e950-efb0-41ed-9103-ced24d7dc4e2}">
-  <dimension ref="A5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0" topLeftCell="A1"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
-  <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="157.703125" collapsed="true"/>
-  </cols>
-  <sheetData>
-    <row r="5" spans="1:1" ht="23.25" customHeight="1">
-      <c r="A5" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>